<commit_message>
updated G4 of Mavs Timberwolves game
</commit_message>
<xml_diff>
--- a/NBA DATA.xlsx
+++ b/NBA DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfens\Documents\STAT400\NBA-Playoff-Stat-Pred\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C8E1F0-15E6-4EEF-BD0E-230CEF4C3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC43D2D2-A7EF-46D4-B41D-6D2B27314286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11352" yWindow="144" windowWidth="11688" windowHeight="12096" xr2:uid="{CC183DD1-A0C6-43B3-866B-AE5C4D2C46C4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC183DD1-A0C6-43B3-866B-AE5C4D2C46C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="27">
   <si>
     <t>Player</t>
   </si>
@@ -488,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34990CCC-45AE-4EC6-BB58-23AD10A04A37}">
-  <dimension ref="A1:K269"/>
+  <dimension ref="A1:K270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I84" sqref="I84:K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3024,6 +3024,41 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85">
+        <v>16</v>
+      </c>
+      <c r="C85">
+        <v>3</v>
+      </c>
+      <c r="D85">
+        <v>4</v>
+      </c>
+      <c r="E85">
+        <v>28</v>
+      </c>
+      <c r="F85">
+        <v>15</v>
+      </c>
+      <c r="G85">
+        <v>10</v>
+      </c>
+      <c r="H85">
+        <v>4</v>
+      </c>
+      <c r="I85">
+        <v>33.9</v>
+      </c>
+      <c r="J85">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K85">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>12</v>
@@ -3549,6 +3584,41 @@
         <v>5.2</v>
       </c>
     </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104">
+        <v>16</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <v>4</v>
+      </c>
+      <c r="E104">
+        <v>16</v>
+      </c>
+      <c r="F104">
+        <v>2</v>
+      </c>
+      <c r="G104">
+        <v>4</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="I104">
+        <v>25.6</v>
+      </c>
+      <c r="J104">
+        <v>5</v>
+      </c>
+      <c r="K104">
+        <v>5.2</v>
+      </c>
+    </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>13</v>
@@ -4074,6 +4144,41 @@
         <v>1.9</v>
       </c>
     </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>13</v>
+      </c>
+      <c r="B123">
+        <v>16</v>
+      </c>
+      <c r="C123">
+        <v>3</v>
+      </c>
+      <c r="D123">
+        <v>4</v>
+      </c>
+      <c r="E123">
+        <v>10</v>
+      </c>
+      <c r="F123">
+        <v>5</v>
+      </c>
+      <c r="G123">
+        <v>2</v>
+      </c>
+      <c r="H123">
+        <v>2</v>
+      </c>
+      <c r="I123">
+        <v>12.9</v>
+      </c>
+      <c r="J123">
+        <v>5.6</v>
+      </c>
+      <c r="K123">
+        <v>1.9</v>
+      </c>
+    </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>14</v>
@@ -4599,6 +4704,41 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>14</v>
+      </c>
+      <c r="B142">
+        <v>16</v>
+      </c>
+      <c r="C142">
+        <v>3</v>
+      </c>
+      <c r="D142">
+        <v>4</v>
+      </c>
+      <c r="E142" t="s">
+        <v>22</v>
+      </c>
+      <c r="F142" t="s">
+        <v>22</v>
+      </c>
+      <c r="G142" t="s">
+        <v>22</v>
+      </c>
+      <c r="H142" t="s">
+        <v>22</v>
+      </c>
+      <c r="I142">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J142">
+        <v>6.9</v>
+      </c>
+      <c r="K142">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>15</v>
@@ -5124,6 +5264,41 @@
         <v>1.6</v>
       </c>
     </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>15</v>
+      </c>
+      <c r="B161">
+        <v>16</v>
+      </c>
+      <c r="C161">
+        <v>3</v>
+      </c>
+      <c r="D161">
+        <v>4</v>
+      </c>
+      <c r="E161">
+        <v>12</v>
+      </c>
+      <c r="F161">
+        <v>8</v>
+      </c>
+      <c r="G161">
+        <v>1</v>
+      </c>
+      <c r="H161">
+        <v>0</v>
+      </c>
+      <c r="I161">
+        <v>11</v>
+      </c>
+      <c r="J161">
+        <v>7.6</v>
+      </c>
+      <c r="K161">
+        <v>1.6</v>
+      </c>
+    </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>16</v>
@@ -5649,6 +5824,41 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>16</v>
+      </c>
+      <c r="B180">
+        <v>16</v>
+      </c>
+      <c r="C180">
+        <v>3</v>
+      </c>
+      <c r="D180">
+        <v>4</v>
+      </c>
+      <c r="E180">
+        <v>5</v>
+      </c>
+      <c r="F180">
+        <v>1</v>
+      </c>
+      <c r="G180">
+        <v>1</v>
+      </c>
+      <c r="H180">
+        <v>1</v>
+      </c>
+      <c r="I180">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J180">
+        <v>3.2</v>
+      </c>
+      <c r="K180">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>17</v>
@@ -6139,6 +6349,41 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>17</v>
+      </c>
+      <c r="B198">
+        <v>15</v>
+      </c>
+      <c r="C198">
+        <v>3</v>
+      </c>
+      <c r="D198">
+        <v>4</v>
+      </c>
+      <c r="E198">
+        <v>29</v>
+      </c>
+      <c r="F198">
+        <v>10</v>
+      </c>
+      <c r="G198">
+        <v>9</v>
+      </c>
+      <c r="H198">
+        <v>2</v>
+      </c>
+      <c r="I198">
+        <v>25.9</v>
+      </c>
+      <c r="J198">
+        <v>5.4</v>
+      </c>
+      <c r="K198">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>18</v>
@@ -6629,6 +6874,41 @@
         <v>3</v>
       </c>
     </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>18</v>
+      </c>
+      <c r="B216">
+        <v>15</v>
+      </c>
+      <c r="C216">
+        <v>3</v>
+      </c>
+      <c r="D216">
+        <v>4</v>
+      </c>
+      <c r="E216">
+        <v>25</v>
+      </c>
+      <c r="F216">
+        <v>5</v>
+      </c>
+      <c r="G216">
+        <v>1</v>
+      </c>
+      <c r="H216">
+        <v>4</v>
+      </c>
+      <c r="I216">
+        <v>21.8</v>
+      </c>
+      <c r="J216">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K216">
+        <v>3</v>
+      </c>
+    </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>19</v>
@@ -7119,6 +7399,41 @@
         <v>1.4</v>
       </c>
     </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>19</v>
+      </c>
+      <c r="B234">
+        <v>15</v>
+      </c>
+      <c r="C234">
+        <v>3</v>
+      </c>
+      <c r="D234">
+        <v>4</v>
+      </c>
+      <c r="E234">
+        <v>10</v>
+      </c>
+      <c r="F234">
+        <v>1</v>
+      </c>
+      <c r="G234">
+        <v>0</v>
+      </c>
+      <c r="H234">
+        <v>2</v>
+      </c>
+      <c r="I234">
+        <v>10.5</v>
+      </c>
+      <c r="J234">
+        <v>3.1</v>
+      </c>
+      <c r="K234">
+        <v>1.4</v>
+      </c>
+    </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>20</v>
@@ -7609,6 +7924,41 @@
         <v>1.3</v>
       </c>
     </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>20</v>
+      </c>
+      <c r="B252">
+        <v>15</v>
+      </c>
+      <c r="C252">
+        <v>3</v>
+      </c>
+      <c r="D252">
+        <v>4</v>
+      </c>
+      <c r="E252">
+        <v>13</v>
+      </c>
+      <c r="F252">
+        <v>10</v>
+      </c>
+      <c r="G252">
+        <v>1</v>
+      </c>
+      <c r="H252">
+        <v>0</v>
+      </c>
+      <c r="I252">
+        <v>14</v>
+      </c>
+      <c r="J252">
+        <v>12.9</v>
+      </c>
+      <c r="K252">
+        <v>1.3</v>
+      </c>
+    </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>21</v>
@@ -8093,10 +8443,45 @@
         <v>11.4</v>
       </c>
       <c r="J269">
-        <v>2.9</v>
+        <v>11.4</v>
       </c>
       <c r="K269">
-        <v>5.9</v>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>21</v>
+      </c>
+      <c r="B270">
+        <v>15</v>
+      </c>
+      <c r="C270">
+        <v>3</v>
+      </c>
+      <c r="D270">
+        <v>4</v>
+      </c>
+      <c r="E270">
+        <v>14</v>
+      </c>
+      <c r="F270">
+        <v>3</v>
+      </c>
+      <c r="G270">
+        <v>7</v>
+      </c>
+      <c r="H270">
+        <v>1</v>
+      </c>
+      <c r="I270">
+        <v>11.4</v>
+      </c>
+      <c r="J270">
+        <v>11.4</v>
+      </c>
+      <c r="K270">
+        <v>11.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>